<commit_message>
improved tables, figures, conferences and 2,3
</commit_message>
<xml_diff>
--- a/abstract/table_Specification.xlsx
+++ b/abstract/table_Specification.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Vehicle dimension</t>
   </si>
@@ -63,10 +63,6 @@
   </si>
   <si>
     <t>CAMERA D435</t>
-  </si>
-  <si>
-    <t>DC12[V],
-Dynamixel XM430-W350-R</t>
   </si>
   <si>
     <t>HOKUYO 2DLidar UTM30LX,
@@ -78,20 +74,30 @@
 Laptop</t>
   </si>
   <si>
-    <t>400[mm]×350[mm]×240[mm]
+    <t>400[mm]×350[mm]×240[mm]</t>
+  </si>
+  <si>
+    <t>INTEL REALSENSE DEPTH</t>
+  </si>
+  <si>
+    <t>ALIENWARE 13 GAMING</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>DC12V,
+Dynamixel XM430-W350-R</t>
+  </si>
+  <si>
+    <t>Two 6.6V Li-Fe Batteries</t>
+  </si>
+  <si>
+    <t>Approx. 13 kg including computer</t>
+  </si>
+  <si>
+    <t>Approx. 400 mm×350 mm×240 mm
 Body only</t>
-  </si>
-  <si>
-    <t>400[mm]×350[mm]×240[mm]</t>
-  </si>
-  <si>
-    <t>INTEL REALSENSE DEPTH</t>
-  </si>
-  <si>
-    <t>ALIENWARE 13 GAMING</t>
-  </si>
-  <si>
-    <t>Laptop</t>
   </si>
 </sst>
 </file>
@@ -209,6 +215,16 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -218,16 +234,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -525,105 +531,105 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="17"/>
+      <c r="D3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="17"/>
+      <c r="D6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="17"/>
+        <v>20</v>
+      </c>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="11"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
+      <c r="C12" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="16" spans="2:5" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="16" spans="2:5" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="17" spans="3:4" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="11"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="3" t="s">
         <v>6</v>
       </c>
@@ -645,7 +651,7 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="3:4" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -653,13 +659,13 @@
       </c>
     </row>
     <row r="22" spans="3:4" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="11"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="11"/>
+      <c r="C23" s="15"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
@@ -670,24 +676,24 @@
       </c>
     </row>
     <row r="25" spans="3:4" ht="2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="11"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="11"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="11"/>
+      <c r="C28" s="15"/>
       <c r="D28" s="7" t="s">
         <v>12</v>
       </c>
@@ -697,17 +703,17 @@
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="3:4" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="3:4" ht="11.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="11"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>